<commit_message>
corrigiendo el error con la grafica
</commit_message>
<xml_diff>
--- a/static/download/admin/Reporte General.xlsx
+++ b/static/download/admin/Reporte General.xlsx
@@ -19,13 +19,13 @@
     <t>SERVICIO SECA S.A DE C.V</t>
   </si>
   <si>
-    <t>Fecha: 26/11/2014</t>
+    <t>Fecha: 28/11/2014</t>
   </si>
   <si>
     <t>REPORTE GENERAL.</t>
   </si>
   <si>
-    <t>Del 18/11/2014 0:00:00 hrs. AL 26/11/2014 23:59:59 hrs.</t>
+    <t>Del 18/11/2014 0:00:00 hrs. AL 28/11/2014 23:59:59 hrs.</t>
   </si>
   <si>
     <t>Tarifa</t>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reporte de ventas" displayName="Reporte de ventas" ref="C10:E13" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reporte de ventas" displayName="Reporte de ventas" ref="C10:E14" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" name="Column2" dataDxfId="1"/>
@@ -520,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:F17"/>
+  <dimension ref="A4:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -604,26 +604,37 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2"/>
+    <row r="14" spans="1:6">
+      <c r="C14" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4">
-        <v>764</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3">
-        <v>2296</v>
+      <c r="D18" s="3">
+        <v>2302.5</v>
       </c>
     </row>
   </sheetData>
@@ -632,7 +643,7 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>